<commit_message>
Single round pins in BOM
</commit_message>
<xml_diff>
--- a/1541_VIA_Parallel_Adapter_lowP/Rev. 0/Excel/VIA_PAR_Adapter_LowP_BOM_v0_0.xlsx
+++ b/1541_VIA_Parallel_Adapter_lowP/Rev. 0/Excel/VIA_PAR_Adapter_LowP_BOM_v0_0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Projekte\_Eigene\C64-Projects\1541-Parallel2UP\1541_VIA_Parallel_Adapter_lowP\Rev. 0\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81CA1CB-D4AA-4DF3-BC7A-8E90F58D16DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49AEAE39-25B2-4D88-81A3-24D991C547BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11184" yWindow="2880" windowWidth="18420" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9348" yWindow="1524" windowWidth="18420" windowHeight="14400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stückliste" sheetId="1" r:id="rId1"/>
@@ -101,26 +101,32 @@
     <t>10p IDC receptacle, 2,54mm</t>
   </si>
   <si>
-    <t>Dual In Line precision round pin Socket, e.g. Reichelt: GS40P (the 2nd socket is for alignment)</t>
-  </si>
-  <si>
     <t>Tyco/AMP or MPE Garry 369-1-010, e.g. Reichelt MPE 369-1-010</t>
   </si>
   <si>
     <t>Tyco/AMP (IDC connector) or MPE Garry 372-1-010, , e.g. Reichelt MPE 372-1-010</t>
+  </si>
+  <si>
+    <t>Dual In Line precision round pin Socket, e.g. Reichelt: GS40P (the 2nd socket is for alignment), single pins: Connfly  DS1005-09-468, tme.eu: STS-1P</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Futura Lt BT"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -586,49 +592,49 @@
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -636,10 +642,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -651,14 +657,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -666,17 +675,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1177,7 +1186,7 @@
   <dimension ref="A1:F148"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1191,24 +1200,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
     </row>
     <row r="3" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -1237,7 +1246,7 @@
       <c r="B4" s="3">
         <v>1</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="13" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -1246,11 +1255,11 @@
       <c r="E4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" s="6" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <f>A4+1</f>
         <v>2</v>
@@ -1267,8 +1276,8 @@
       <c r="E5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="15" t="s">
-        <v>25</v>
+      <c r="F5" s="17" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -1279,17 +1288,17 @@
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>26</v>
+      <c r="F6" s="13" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -1297,20 +1306,20 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="13">
         <v>1</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="15" t="s">
-        <v>27</v>
+      <c r="F7" s="13" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="6" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
@@ -1321,7 +1330,7 @@
       <c r="B8" s="3">
         <v>1</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="13" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="4"/>
@@ -1343,7 +1352,7 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="13" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>